<commit_message>
Opgeschoonde data met verzamelingen
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Voorkeur gang</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Koppel blijft bijelkaar</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -485,6 +490,9 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -508,6 +516,9 @@
         <v>8</v>
       </c>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -531,6 +542,9 @@
         <v>8</v>
       </c>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -554,6 +568,9 @@
         <v>6</v>
       </c>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -577,6 +594,9 @@
         <v>6</v>
       </c>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -600,6 +620,9 @@
         <v>8</v>
       </c>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -623,6 +646,9 @@
         <v>8</v>
       </c>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -644,6 +670,9 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -665,6 +694,9 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -692,6 +724,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -715,6 +750,9 @@
         <v>8</v>
       </c>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -742,6 +780,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -765,6 +806,9 @@
         <v>8</v>
       </c>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -792,6 +836,9 @@
           <t>Na</t>
         </is>
       </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -815,6 +862,9 @@
         <v>8</v>
       </c>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -838,6 +888,9 @@
         <v>8</v>
       </c>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -861,6 +914,9 @@
         <v>8</v>
       </c>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -888,6 +944,9 @@
           <t>Na</t>
         </is>
       </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -909,6 +968,9 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -936,6 +998,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -957,6 +1022,9 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -980,6 +1048,9 @@
         <v>6</v>
       </c>
       <c r="G23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1003,6 +1074,9 @@
         <v>8</v>
       </c>
       <c r="G24" t="inlineStr"/>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1026,6 +1100,9 @@
         <v>8</v>
       </c>
       <c r="G25" t="inlineStr"/>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1049,6 +1126,9 @@
         <v>8</v>
       </c>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1072,6 +1152,9 @@
         <v>8</v>
       </c>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1095,6 +1178,9 @@
         <v>8</v>
       </c>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1118,6 +1204,9 @@
         <v>8</v>
       </c>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1141,6 +1230,9 @@
         <v>6</v>
       </c>
       <c r="G30" t="inlineStr"/>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1164,6 +1256,9 @@
         <v>8</v>
       </c>
       <c r="G31" t="inlineStr"/>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1187,6 +1282,9 @@
         <v>8</v>
       </c>
       <c r="G32" t="inlineStr"/>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1210,6 +1308,9 @@
         <v>8</v>
       </c>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1233,6 +1334,9 @@
         <v>8</v>
       </c>
       <c r="G34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1254,6 +1358,9 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1281,6 +1388,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1304,6 +1414,9 @@
         <v>8</v>
       </c>
       <c r="G37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1327,6 +1440,9 @@
         <v>8</v>
       </c>
       <c r="G38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1350,6 +1466,9 @@
         <v>8</v>
       </c>
       <c r="G39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1373,6 +1492,9 @@
         <v>6</v>
       </c>
       <c r="G40" t="inlineStr"/>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1400,6 +1522,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1421,6 +1546,9 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1444,6 +1572,9 @@
         <v>8</v>
       </c>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1467,6 +1598,9 @@
         <v>8</v>
       </c>
       <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1490,6 +1624,9 @@
         <v>6</v>
       </c>
       <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1513,6 +1650,9 @@
         <v>6</v>
       </c>
       <c r="G46" t="inlineStr"/>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1536,6 +1676,9 @@
         <v>6</v>
       </c>
       <c r="G47" t="inlineStr"/>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1559,6 +1702,9 @@
         <v>8</v>
       </c>
       <c r="G48" t="inlineStr"/>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1582,6 +1728,9 @@
         <v>6</v>
       </c>
       <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1603,6 +1752,9 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1626,6 +1778,9 @@
         <v>8</v>
       </c>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1649,6 +1804,9 @@
         <v>8</v>
       </c>
       <c r="G52" t="inlineStr"/>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1670,6 +1828,9 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1697,6 +1858,9 @@
           <t>Na</t>
         </is>
       </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1720,6 +1884,9 @@
         <v>8</v>
       </c>
       <c r="G55" t="inlineStr"/>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1743,6 +1910,9 @@
         <v>6</v>
       </c>
       <c r="G56" t="inlineStr"/>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1766,6 +1936,9 @@
         <v>8</v>
       </c>
       <c r="G57" t="inlineStr"/>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1789,6 +1962,9 @@
         <v>8</v>
       </c>
       <c r="G58" t="inlineStr"/>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1812,6 +1988,9 @@
         <v>6</v>
       </c>
       <c r="G59" t="inlineStr"/>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1833,6 +2012,9 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1856,6 +2038,9 @@
         <v>8</v>
       </c>
       <c r="G61" t="inlineStr"/>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1879,6 +2064,9 @@
         <v>8</v>
       </c>
       <c r="G62" t="inlineStr"/>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1902,6 +2090,9 @@
         <v>8</v>
       </c>
       <c r="G63" t="inlineStr"/>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1925,6 +2116,9 @@
         <v>6</v>
       </c>
       <c r="G64" t="inlineStr"/>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1948,6 +2142,9 @@
         <v>8</v>
       </c>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1971,6 +2168,9 @@
         <v>8</v>
       </c>
       <c r="G66" t="inlineStr"/>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1994,6 +2194,9 @@
         <v>8</v>
       </c>
       <c r="G67" t="inlineStr"/>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2017,6 +2220,9 @@
         <v>8</v>
       </c>
       <c r="G68" t="inlineStr"/>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2040,6 +2246,9 @@
         <v>7</v>
       </c>
       <c r="G69" t="inlineStr"/>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2063,6 +2272,9 @@
         <v>8</v>
       </c>
       <c r="G70" t="inlineStr"/>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2086,6 +2298,9 @@
         <v>8</v>
       </c>
       <c r="G71" t="inlineStr"/>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2109,6 +2324,9 @@
         <v>8</v>
       </c>
       <c r="G72" t="inlineStr"/>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2132,6 +2350,9 @@
         <v>8</v>
       </c>
       <c r="G73" t="inlineStr"/>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2155,6 +2376,9 @@
         <v>8</v>
       </c>
       <c r="G74" t="inlineStr"/>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2178,6 +2402,9 @@
         <v>8</v>
       </c>
       <c r="G75" t="inlineStr"/>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2201,6 +2428,9 @@
         <v>8</v>
       </c>
       <c r="G76" t="inlineStr"/>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2224,6 +2454,9 @@
         <v>8</v>
       </c>
       <c r="G77" t="inlineStr"/>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2247,6 +2480,9 @@
         <v>8</v>
       </c>
       <c r="G78" t="inlineStr"/>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2274,6 +2510,9 @@
           <t>Hoofd</t>
         </is>
       </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2297,6 +2536,9 @@
         <v>8</v>
       </c>
       <c r="G80" t="inlineStr"/>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2320,6 +2562,9 @@
         <v>8</v>
       </c>
       <c r="G81" t="inlineStr"/>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2343,6 +2588,9 @@
         <v>8</v>
       </c>
       <c r="G82" t="inlineStr"/>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2364,6 +2612,9 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
+      <c r="H83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2387,6 +2638,9 @@
         <v>8</v>
       </c>
       <c r="G84" t="inlineStr"/>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2410,6 +2664,9 @@
         <v>8</v>
       </c>
       <c r="G85" t="inlineStr"/>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2437,6 +2694,9 @@
           <t>Na</t>
         </is>
       </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2460,6 +2720,9 @@
         <v>6</v>
       </c>
       <c r="G87" t="inlineStr"/>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2483,6 +2746,9 @@
         <v>6</v>
       </c>
       <c r="G88" t="inlineStr"/>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2506,6 +2772,9 @@
         <v>8</v>
       </c>
       <c r="G89" t="inlineStr"/>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2529,6 +2798,9 @@
         <v>8</v>
       </c>
       <c r="G90" t="inlineStr"/>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2552,6 +2824,9 @@
         <v>8</v>
       </c>
       <c r="G91" t="inlineStr"/>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2573,6 +2848,9 @@
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2596,6 +2874,9 @@
         <v>8</v>
       </c>
       <c r="G93" t="inlineStr"/>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2619,6 +2900,9 @@
         <v>8</v>
       </c>
       <c r="G94" t="inlineStr"/>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -2640,6 +2924,9 @@
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
+      <c r="H95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2661,6 +2948,9 @@
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
+      <c r="H96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2688,6 +2978,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -2711,6 +3004,9 @@
         <v>8</v>
       </c>
       <c r="G98" t="inlineStr"/>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -2738,6 +3034,9 @@
           <t>Voor</t>
         </is>
       </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -2761,6 +3060,9 @@
         <v>6</v>
       </c>
       <c r="G100" t="inlineStr"/>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -2784,6 +3086,9 @@
         <v>8</v>
       </c>
       <c r="G101" t="inlineStr"/>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -2807,6 +3112,9 @@
         <v>8</v>
       </c>
       <c r="G102" t="inlineStr"/>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -2830,6 +3138,9 @@
         <v>8</v>
       </c>
       <c r="G103" t="inlineStr"/>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -2853,6 +3164,9 @@
         <v>8</v>
       </c>
       <c r="G104" t="inlineStr"/>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -2876,6 +3190,9 @@
         <v>8</v>
       </c>
       <c r="G105" t="inlineStr"/>
+      <c r="H105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -2899,6 +3216,9 @@
         <v>8</v>
       </c>
       <c r="G106" t="inlineStr"/>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -2926,6 +3246,9 @@
           <t>Na</t>
         </is>
       </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -2949,6 +3272,9 @@
         <v>8</v>
       </c>
       <c r="G108" t="inlineStr"/>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -2972,6 +3298,9 @@
         <v>8</v>
       </c>
       <c r="G109" t="inlineStr"/>
+      <c r="H109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -2995,6 +3324,9 @@
         <v>8</v>
       </c>
       <c r="G110" t="inlineStr"/>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3018,6 +3350,9 @@
         <v>6</v>
       </c>
       <c r="G111" t="inlineStr"/>
+      <c r="H111" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
JA! DE GANGEN VAN VORIG JAAR STAAN ER IN
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Koppel blijft bijelkaar</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Vorig jaar gang</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -493,6 +498,7 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -519,6 +525,7 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -545,6 +552,7 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -571,6 +579,11 @@
       <c r="H5" t="n">
         <v>0</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -597,6 +610,11 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -623,6 +641,11 @@
       <c r="H7" t="n">
         <v>0</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -649,6 +672,7 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -673,6 +697,7 @@
       <c r="H9" t="n">
         <v>0</v>
       </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -697,6 +722,7 @@
       <c r="H10" t="n">
         <v>0</v>
       </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -727,6 +753,7 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -753,6 +780,7 @@
       <c r="H12" t="n">
         <v>0</v>
       </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -783,6 +811,11 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -809,6 +842,11 @@
       <c r="H14" t="n">
         <v>0</v>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -839,6 +877,11 @@
       <c r="H15" t="n">
         <v>0</v>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -865,6 +908,11 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -891,6 +939,11 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -917,6 +970,11 @@
       <c r="H18" t="n">
         <v>0</v>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -946,6 +1004,11 @@
       </c>
       <c r="H19" t="n">
         <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -971,6 +1034,11 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1001,6 +1069,7 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1025,6 +1094,7 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1051,6 +1121,11 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1077,6 +1152,11 @@
       <c r="H24" t="n">
         <v>0</v>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1103,6 +1183,11 @@
       <c r="H25" t="n">
         <v>0</v>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1129,6 +1214,11 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1155,6 +1245,7 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1181,6 +1272,11 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1207,6 +1303,7 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1233,6 +1330,11 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1259,6 +1361,11 @@
       <c r="H31" t="n">
         <v>0</v>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1285,6 +1392,7 @@
       <c r="H32" t="n">
         <v>0</v>
       </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1311,6 +1419,11 @@
       <c r="H33" t="n">
         <v>0</v>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1337,6 +1450,7 @@
       <c r="H34" t="n">
         <v>0</v>
       </c>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1361,6 +1475,7 @@
       <c r="H35" t="n">
         <v>0</v>
       </c>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1391,6 +1506,7 @@
       <c r="H36" t="n">
         <v>0</v>
       </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1417,6 +1533,7 @@
       <c r="H37" t="n">
         <v>0</v>
       </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1443,6 +1560,11 @@
       <c r="H38" t="n">
         <v>0</v>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1469,6 +1591,11 @@
       <c r="H39" t="n">
         <v>0</v>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1495,6 +1622,7 @@
       <c r="H40" t="n">
         <v>0</v>
       </c>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1524,6 +1652,11 @@
       </c>
       <c r="H41" t="n">
         <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1549,6 +1682,7 @@
       <c r="H42" t="n">
         <v>0</v>
       </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1575,6 +1709,11 @@
       <c r="H43" t="n">
         <v>0</v>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1601,6 +1740,7 @@
       <c r="H44" t="n">
         <v>0</v>
       </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1627,6 +1767,11 @@
       <c r="H45" t="n">
         <v>0</v>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1653,6 +1798,11 @@
       <c r="H46" t="n">
         <v>0</v>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1679,6 +1829,11 @@
       <c r="H47" t="n">
         <v>0</v>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1705,6 +1860,11 @@
       <c r="H48" t="n">
         <v>0</v>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1730,6 +1890,11 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
         <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1755,6 +1920,11 @@
       <c r="H50" t="n">
         <v>0</v>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1781,6 +1951,7 @@
       <c r="H51" t="n">
         <v>0</v>
       </c>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1806,6 +1977,11 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
         <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -1831,6 +2007,7 @@
       <c r="H53" t="n">
         <v>0</v>
       </c>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1861,6 +2038,11 @@
       <c r="H54" t="n">
         <v>0</v>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1887,6 +2069,11 @@
       <c r="H55" t="n">
         <v>0</v>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1913,6 +2100,11 @@
       <c r="H56" t="n">
         <v>0</v>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1939,6 +2131,11 @@
       <c r="H57" t="n">
         <v>0</v>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1965,6 +2162,7 @@
       <c r="H58" t="n">
         <v>0</v>
       </c>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1990,6 +2188,11 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
         <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -2015,6 +2218,7 @@
       <c r="H60" t="n">
         <v>0</v>
       </c>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2041,6 +2245,7 @@
       <c r="H61" t="n">
         <v>0</v>
       </c>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2067,6 +2272,7 @@
       <c r="H62" t="n">
         <v>0</v>
       </c>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2093,6 +2299,11 @@
       <c r="H63" t="n">
         <v>0</v>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2119,6 +2330,11 @@
       <c r="H64" t="n">
         <v>0</v>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2145,6 +2361,11 @@
       <c r="H65" t="n">
         <v>0</v>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2171,6 +2392,7 @@
       <c r="H66" t="n">
         <v>0</v>
       </c>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2197,6 +2419,11 @@
       <c r="H67" t="n">
         <v>0</v>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2223,6 +2450,11 @@
       <c r="H68" t="n">
         <v>0</v>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2249,6 +2481,7 @@
       <c r="H69" t="n">
         <v>0</v>
       </c>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2275,6 +2508,7 @@
       <c r="H70" t="n">
         <v>0</v>
       </c>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2301,6 +2535,11 @@
       <c r="H71" t="n">
         <v>0</v>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2327,6 +2566,7 @@
       <c r="H72" t="n">
         <v>0</v>
       </c>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2353,6 +2593,11 @@
       <c r="H73" t="n">
         <v>0</v>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2379,6 +2624,11 @@
       <c r="H74" t="n">
         <v>0</v>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2405,6 +2655,11 @@
       <c r="H75" t="n">
         <v>0</v>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2431,6 +2686,11 @@
       <c r="H76" t="n">
         <v>0</v>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2457,6 +2717,11 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2483,6 +2748,11 @@
       <c r="H78" t="n">
         <v>0</v>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2513,6 +2783,7 @@
       <c r="H79" t="n">
         <v>0</v>
       </c>
+      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2539,6 +2810,7 @@
       <c r="H80" t="n">
         <v>0</v>
       </c>
+      <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2565,6 +2837,11 @@
       <c r="H81" t="n">
         <v>0</v>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2590,6 +2867,11 @@
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
         <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -2615,6 +2897,7 @@
       <c r="H83" t="n">
         <v>1</v>
       </c>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2641,6 +2924,11 @@
       <c r="H84" t="n">
         <v>0</v>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2667,6 +2955,7 @@
       <c r="H85" t="n">
         <v>0</v>
       </c>
+      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2697,6 +2986,11 @@
       <c r="H86" t="n">
         <v>0</v>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2723,6 +3017,7 @@
       <c r="H87" t="n">
         <v>0</v>
       </c>
+      <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2749,6 +3044,11 @@
       <c r="H88" t="n">
         <v>0</v>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2775,6 +3075,11 @@
       <c r="H89" t="n">
         <v>0</v>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2801,6 +3106,11 @@
       <c r="H90" t="n">
         <v>0</v>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2827,6 +3137,7 @@
       <c r="H91" t="n">
         <v>0</v>
       </c>
+      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -2851,6 +3162,7 @@
       <c r="H92" t="n">
         <v>0</v>
       </c>
+      <c r="I92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -2877,6 +3189,11 @@
       <c r="H93" t="n">
         <v>0</v>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -2902,6 +3219,11 @@
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
         <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
       </c>
     </row>
     <row r="95">
@@ -2927,6 +3249,7 @@
       <c r="H95" t="n">
         <v>1</v>
       </c>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -2951,6 +3274,7 @@
       <c r="H96" t="n">
         <v>1</v>
       </c>
+      <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -2981,6 +3305,7 @@
       <c r="H97" t="n">
         <v>0</v>
       </c>
+      <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -3007,6 +3332,11 @@
       <c r="H98" t="n">
         <v>0</v>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -3037,6 +3367,7 @@
       <c r="H99" t="n">
         <v>0</v>
       </c>
+      <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3063,6 +3394,11 @@
       <c r="H100" t="n">
         <v>0</v>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -3089,6 +3425,11 @@
       <c r="H101" t="n">
         <v>0</v>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -3115,6 +3456,7 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3141,6 +3483,11 @@
       <c r="H103" t="n">
         <v>0</v>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3167,6 +3514,11 @@
       <c r="H104" t="n">
         <v>0</v>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3193,6 +3545,11 @@
       <c r="H105" t="n">
         <v>0</v>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3219,6 +3576,11 @@
       <c r="H106" t="n">
         <v>0</v>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3249,6 +3611,11 @@
       <c r="H107" t="n">
         <v>0</v>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3275,6 +3642,11 @@
       <c r="H108" t="n">
         <v>0</v>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3301,6 +3673,11 @@
       <c r="H109" t="n">
         <v>0</v>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Voor</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3327,6 +3704,7 @@
       <c r="H110" t="n">
         <v>0</v>
       </c>
+      <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3352,6 +3730,11 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
         <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>